<commit_message>
Syncing back up with server
</commit_message>
<xml_diff>
--- a/resources/assets/files/Alopecia-Treatment-Actionable-Insights.xlsx
+++ b/resources/assets/files/Alopecia-Treatment-Actionable-Insights.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\XAMPP\htdocs\brettjaybrewster\homebase\resources\assets\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\seal-file2\User Folders\bbrewster\Desktop\Development\local-workspace\bjb\homebase\resources\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270F8C67-5E6A-44FE-B8B9-FE3A9EC8EC9B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE86F933-4970-4A5D-BE1E-897E7AEA9084}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{C3F0902A-DD7D-41B2-BCEE-024CD922F4CF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C3F0902A-DD7D-41B2-BCEE-024CD922F4CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
   <si>
     <t>Alopecia Treatment Analysis</t>
   </si>
@@ -78,9 +78,15 @@
     <t>Aromatherapy</t>
   </si>
   <si>
+    <t>Create oil blend based on study and apply twice daily.</t>
+  </si>
+  <si>
     <t>Occassional 24+ Hr Fasts</t>
   </si>
   <si>
+    <t>Occasionally (1x/wk or 1x/month) fast for 24+ hours (Nothing other than water)</t>
+  </si>
+  <si>
     <t>Consume &lt;25g sugar/day</t>
   </si>
   <si>
@@ -118,6 +124,9 @@
   </si>
   <si>
     <t>TRACK</t>
+  </si>
+  <si>
+    <t>Track everything consumed. Integrate with APIs ideally to pull in as much info as possible. Would allow for tracking of macros, micros, time restricted eating window, etc. Time est ~20 hours to develop + 2 min per meal</t>
   </si>
   <si>
     <t>Brew own Kombucha</t>
@@ -284,35 +293,12 @@
   <si>
     <t>Research, Purchase, and use daily. 2 Hours of research and then 2 min/day to refill</t>
   </si>
-  <si>
-    <t>Occasionally (1x/wk or 1x/month) fast for 24+ hours (Nothing other than water)
-Maximum benefit may not be achieved until 36-72+ hours</t>
-  </si>
-  <si>
-    <t>Use Cronometer to track consumption</t>
-  </si>
-  <si>
-    <t>0+</t>
-  </si>
-  <si>
-    <t>Track everything consumed using already reputable app. Will require substantially less up-front time and can tie into things that would take forever to setup. Time est ~3 hours to familiarize self with software and setup correct data and tracking metrics; then 5 min per day.</t>
-  </si>
-  <si>
-    <t>Track everything consumed. Integrate with APIs ideally to pull in as much info as possible. Would allow for tracking of macros, micros, time restricted eating window, etc. Time est ~30 hours to develop + 2 min per meal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Based on study:
-- Research aromatherapy techniques on YouTube [20m]
-- Create oil: Thyme vulgaris (2 drops, 88 mg), Lavandula agustifolia (3 drops, 108 mg), Rosmarinus officinalis (3 drops, 114 mg), and Cedrus atlantica (2 drops, 94 mg). These oils were mixed in a carrier oil, which was a combination of jojoba, 3 mL, and grapeseed, 20 mL, oils. [10m] x 6 times/year 
-- Massage oil into the scalp for a minimum of 2 minutes every night. Wrap a warm towel around the head to aid absorption of the oils. [2m] x 365
-</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,34 +321,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -377,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -391,30 +356,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -424,11 +365,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <mruColors>
-      <color rgb="FFCCFFCC"/>
-    </mruColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -737,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB3A2EB-1285-48F8-BB2A-0820AFD64185}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,25 +691,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
@@ -782,101 +718,97 @@
         <v>3</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="6">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4">
         <v>4</v>
       </c>
-      <c r="C3" s="7">
-        <v>3</v>
-      </c>
-      <c r="D3" s="7">
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
         <f>(60+(12*30))</f>
         <v>420</v>
       </c>
-      <c r="E3" s="7">
-        <v>0</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="5" t="s">
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <f>(2*2*365)</f>
+        <v>1460</v>
+      </c>
+      <c r="E4" s="1">
+        <v>50</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="6">
-        <v>3</v>
-      </c>
-      <c r="C4" s="7">
-        <v>1</v>
-      </c>
-      <c r="D4" s="6">
-        <f>(20+60+(2*365))</f>
-        <v>810</v>
-      </c>
-      <c r="E4" s="7">
-        <v>50</v>
-      </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="6">
-        <v>3</v>
-      </c>
-      <c r="C5" s="6">
-        <v>3</v>
-      </c>
-      <c r="D5" s="7">
-        <v>0</v>
-      </c>
-      <c r="E5" s="7">
-        <v>0</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="6">
-        <v>3</v>
-      </c>
-      <c r="C6" s="6">
-        <v>3</v>
-      </c>
-      <c r="D6" s="7">
-        <v>0</v>
-      </c>
-      <c r="E6" s="7">
-        <v>0</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="5" t="s">
-        <v>67</v>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B7" s="4">
         <v>3</v>
@@ -892,15 +824,15 @@
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4">
         <v>4</v>
@@ -916,15 +848,15 @@
         <v>210</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B9" s="4">
         <v>4</v>
@@ -941,63 +873,64 @@
         <v>1000</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="6">
-        <v>4</v>
-      </c>
-      <c r="C10" s="6">
-        <v>4</v>
-      </c>
-      <c r="D10" s="7">
-        <f>(300+(5*365))</f>
-        <v>2125</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="10">
-        <v>3</v>
-      </c>
-      <c r="C11" s="10">
-        <v>3</v>
-      </c>
-      <c r="D11" s="10">
-        <f>(1800+(2*3*365))</f>
-        <v>3990</v>
-      </c>
-      <c r="E11" s="11">
-        <v>0</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>71</v>
+      <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="4">
+        <v>3</v>
+      </c>
+      <c r="C10" s="4">
+        <v>3</v>
+      </c>
+      <c r="D10" s="4">
+        <f>(1200+(2*3*365))</f>
+        <v>3390</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="4">
+        <v>3</v>
+      </c>
+      <c r="C11" s="4">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1">
+        <f>(52*15)</f>
+        <v>780</v>
+      </c>
+      <c r="E11" s="1">
+        <f>(-7*26)</f>
+        <v>-182</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B12" s="4">
         <v>3</v>
@@ -1005,96 +938,90 @@
       <c r="C12" s="4">
         <v>3</v>
       </c>
-      <c r="D12" s="1">
-        <f>(52*15)</f>
-        <v>780</v>
-      </c>
-      <c r="E12" s="1">
-        <f>(-7*26)</f>
-        <v>-182</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="6">
-        <v>3</v>
-      </c>
-      <c r="C13" s="6">
-        <v>3</v>
-      </c>
-      <c r="D13" s="6">
+      <c r="D12" s="4">
         <f>(5*365)</f>
         <v>1825</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E12" s="1">
         <f>(-4*26)</f>
         <v>-104</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>24</v>
+      <c r="F12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2</v>
+      </c>
+      <c r="C13" s="4">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="1">
+        <v>35</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="1">
+        <v>31</v>
+      </c>
+      <c r="B14" s="4">
+        <v>3</v>
+      </c>
+      <c r="C14" s="4">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1">
         <v>2</v>
       </c>
-      <c r="C14" s="4">
-        <v>3</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="1">
-        <v>35</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="6">
-        <v>3</v>
-      </c>
-      <c r="C15" s="6">
-        <v>3</v>
-      </c>
-      <c r="D15" s="7">
-        <v>0</v>
-      </c>
-      <c r="E15" s="7">
-        <v>0</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="5" t="s">
-        <v>31</v>
+      <c r="C15" s="4">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B16" s="1">
         <v>2</v>
       </c>
-      <c r="C16" s="4">
-        <v>3</v>
+      <c r="C16" s="1">
+        <v>2</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
@@ -1103,106 +1030,106 @@
         <v>0</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="1">
-        <v>2</v>
+        <v>35</v>
+      </c>
+      <c r="B17" s="4">
+        <v>3</v>
       </c>
       <c r="C17" s="1">
         <v>2</v>
       </c>
       <c r="D17" s="1">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="E17" s="1">
         <v>0</v>
       </c>
+      <c r="F17" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="G17" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="6">
-        <v>3</v>
-      </c>
-      <c r="C18" s="7">
+      <c r="A18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="1">
         <v>2</v>
       </c>
-      <c r="D18" s="7">
-        <v>120</v>
-      </c>
-      <c r="E18" s="7">
-        <v>0</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="7">
-        <v>2</v>
-      </c>
-      <c r="C19" s="6">
-        <v>3</v>
-      </c>
-      <c r="D19" s="7">
+      <c r="C18" s="4">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1">
         <f>(300+(1*365))</f>
         <v>665</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="4">
-        <v>3</v>
-      </c>
-      <c r="C20" s="4">
-        <v>3</v>
-      </c>
-      <c r="D20" s="4">
+      <c r="E18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="4">
+        <v>3</v>
+      </c>
+      <c r="C19" s="4">
+        <v>3</v>
+      </c>
+      <c r="D19" s="4">
         <f>(((365/7)*4)*7)</f>
         <v>1460</v>
       </c>
+      <c r="E19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2</v>
+      </c>
+      <c r="C20" s="4">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
       <c r="E20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="1">
-        <v>2</v>
+        <v>51</v>
+      </c>
+      <c r="B21" s="4">
+        <v>3</v>
       </c>
       <c r="C21" s="4">
         <v>3</v>
@@ -1210,16 +1137,16 @@
       <c r="D21" s="1">
         <v>0</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>47</v>
+      <c r="E21" s="1">
+        <v>0</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B22" s="4">
         <v>3</v>
@@ -1228,67 +1155,71 @@
         <v>3</v>
       </c>
       <c r="D22" s="1">
+        <f>0</f>
         <v>0</v>
       </c>
       <c r="E22" s="1">
-        <v>0</v>
+        <f>(12*10)</f>
+        <v>120</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="4">
-        <v>3</v>
+        <v>55</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2</v>
       </c>
       <c r="C23" s="4">
-        <v>3</v>
-      </c>
-      <c r="D23" s="1">
-        <f>0</f>
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="D23" s="4">
+        <f>ROUND(((365/7)*4)*45, 0)</f>
+        <v>9386</v>
       </c>
       <c r="E23" s="1">
-        <f>(12*10)</f>
-        <v>120</v>
+        <v>0</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="1">
-        <v>2</v>
+        <v>56</v>
+      </c>
+      <c r="B24" s="4">
+        <v>3</v>
       </c>
       <c r="C24" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D24" s="4">
-        <f>ROUND(((365/7)*4)*45, 0)</f>
-        <v>9386</v>
+        <f>ROUND(((365/7)*3)*20, 0)</f>
+        <v>3129</v>
       </c>
       <c r="E24" s="1">
         <v>0</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="4">
-        <v>3</v>
+        <v>59</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2</v>
       </c>
       <c r="C25" s="4">
         <v>3</v>
@@ -1301,15 +1232,15 @@
         <v>0</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="B26" s="1">
         <v>2</v>
@@ -1318,22 +1249,22 @@
         <v>3</v>
       </c>
       <c r="D26" s="4">
-        <f>ROUND(((365/7)*3)*20, 0)</f>
-        <v>3129</v>
+        <f>ROUND(((365/7)*5*8),0)</f>
+        <v>2086</v>
       </c>
       <c r="E26" s="1">
         <v>0</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B27" s="1">
         <v>2</v>
@@ -1342,83 +1273,59 @@
         <v>3</v>
       </c>
       <c r="D27" s="4">
-        <f>ROUND(((365/7)*5*8),0)</f>
-        <v>2086</v>
-      </c>
-      <c r="E27" s="1">
-        <v>0</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" s="1">
-        <v>2</v>
-      </c>
-      <c r="C28" s="4">
-        <v>3</v>
-      </c>
-      <c r="D28" s="4">
         <f>ROUND(((365/7)*4*20),0)</f>
         <v>4171</v>
       </c>
+      <c r="E27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="4">
+        <v>4</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2</v>
+      </c>
+      <c r="D28" s="1">
+        <f>(10*60)</f>
+        <v>600</v>
+      </c>
       <c r="E28" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" s="4">
-        <v>4</v>
+        <v>68</v>
+      </c>
+      <c r="B29" s="1">
+        <v>2</v>
       </c>
       <c r="C29" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D29" s="1">
-        <f>(10*60)</f>
-        <v>600</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B30" s="1">
-        <v>2</v>
-      </c>
-      <c r="C30" s="1">
-        <v>3</v>
-      </c>
-      <c r="D30" s="1">
         <f>(120+(365*2))</f>
         <v>850</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>66</v>
+      <c r="G29" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>